<commit_message>
Generar CSV de productos
Se agrega botón de descargar CSV
Se agregan los campos de SKU y codigoBarras en el formulario de insertar y editar producto
Se agregan las columnas de SKU y codigoBarras en el formato de alta de productos
</commit_message>
<xml_diff>
--- a/CREA3M/assets/productos.xlsx
+++ b/CREA3M/assets/productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\BlueCloud\Proyectos\Crea\crea3M\CREA3M\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\Respaldo\crea3M\CREA3M\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCA5214-B64F-4EB9-9D9D-34BDE2D65E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB44890-BEBC-4D9D-8C93-E8314B738951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3960" windowWidth="22425" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Walmart" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>NP</t>
   </si>
@@ -102,12 +102,24 @@
   <si>
     <t>IdSubcategoria</t>
   </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>CodigoBarras</t>
+  </si>
+  <si>
+    <t>LIJA3349393</t>
+  </si>
+  <si>
+    <t>EX33939932</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -136,6 +148,10 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -250,8 +266,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,19 +277,19 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I323"/>
+  <dimension ref="A1:K323"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="B2:I7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1449,10 +1465,12 @@
     <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="8" max="10" width="10.875" style="1"/>
+    <col min="11" max="11" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1480,8 +1498,14 @@
       <c r="I1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1509,8 +1533,14 @@
       <c r="I2" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="7">
+        <v>60455033344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1538,8 +1568,14 @@
       <c r="I3" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="7">
+        <v>60455033336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1567,8 +1603,12 @@
       <c r="I4" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="15"/>
+      <c r="K4" s="7">
+        <v>60455031405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1596,8 +1636,12 @@
       <c r="I5" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="15"/>
+      <c r="K5" s="7">
+        <v>60455031389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1625,8 +1669,12 @@
       <c r="I6" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="15"/>
+      <c r="K6" s="7">
+        <v>60455033310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1654,8 +1702,12 @@
       <c r="I7" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="15"/>
+      <c r="K7" s="7">
+        <v>60650034972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1665,8 +1717,10 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1676,8 +1730,10 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1687,8 +1743,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1698,8 +1756,10 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1709,8 +1769,10 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1720,8 +1782,10 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1731,8 +1795,10 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1742,8 +1808,10 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1753,8 +1821,10 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1764,8 +1834,10 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1775,8 +1847,10 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1786,8 +1860,10 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1797,8 +1873,10 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1808,8 +1886,10 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1819,8 +1899,10 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1830,8 +1912,10 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1841,8 +1925,10 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1852,8 +1938,10 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1863,8 +1951,10 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1874,8 +1964,10 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1885,8 +1977,10 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1896,8 +1990,10 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1907,8 +2003,10 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1918,8 +2016,10 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1929,8 +2029,10 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1940,8 +2042,10 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1951,8 +2055,10 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1962,8 +2068,10 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1973,8 +2081,10 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -1984,8 +2094,10 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1995,8 +2107,10 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2006,8 +2120,10 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2017,8 +2133,10 @@
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -2028,8 +2146,10 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -2039,8 +2159,10 @@
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2050,8 +2172,10 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2061,8 +2185,10 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2072,8 +2198,10 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -2083,8 +2211,10 @@
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -2094,8 +2224,10 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -2105,8 +2237,10 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -2116,8 +2250,10 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -2127,8 +2263,10 @@
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -2138,8 +2276,10 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+    </row>
+    <row r="52" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -2149,8 +2289,10 @@
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -2160,8 +2302,10 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -2171,8 +2315,10 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -2182,8 +2328,10 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2193,8 +2341,10 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -2204,8 +2354,10 @@
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -2215,8 +2367,10 @@
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -2226,8 +2380,10 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -2237,8 +2393,10 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
-    </row>
-    <row r="61" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -2248,8 +2406,10 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
-    </row>
-    <row r="62" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -2259,8 +2419,10 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
-    </row>
-    <row r="63" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -2270,8 +2432,10 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
-    </row>
-    <row r="64" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -2281,8 +2445,10 @@
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
-    </row>
-    <row r="65" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -2292,8 +2458,10 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
-    </row>
-    <row r="66" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -2303,8 +2471,10 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -2314,8 +2484,10 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
-    </row>
-    <row r="68" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -2325,8 +2497,10 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
-    </row>
-    <row r="69" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -2336,8 +2510,10 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
-    </row>
-    <row r="70" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -2347,8 +2523,10 @@
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -2358,8 +2536,10 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -2369,8 +2549,10 @@
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -2380,8 +2562,10 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -2391,8 +2575,10 @@
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -2402,8 +2588,10 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -2413,8 +2601,10 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -2424,8 +2614,10 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -2435,8 +2627,10 @@
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -2446,8 +2640,10 @@
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -2457,8 +2653,10 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+    </row>
+    <row r="81" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -2468,8 +2666,10 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+    </row>
+    <row r="82" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -2479,8 +2679,10 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+    </row>
+    <row r="83" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -2490,8 +2692,10 @@
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+    </row>
+    <row r="84" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -2501,8 +2705,10 @@
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="7"/>
+      <c r="K84" s="7"/>
+    </row>
+    <row r="85" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -2512,8 +2718,10 @@
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+    </row>
+    <row r="86" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -2523,8 +2731,10 @@
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -2534,8 +2744,10 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+    </row>
+    <row r="88" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -2545,8 +2757,10 @@
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -2556,8 +2770,10 @@
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -2567,8 +2783,10 @@
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -2578,8 +2796,10 @@
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -2589,8 +2809,10 @@
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -2600,8 +2822,10 @@
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -2611,8 +2835,10 @@
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+    </row>
+    <row r="95" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -2622,8 +2848,10 @@
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+    </row>
+    <row r="96" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -2633,8 +2861,10 @@
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J96" s="7"/>
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -2644,8 +2874,10 @@
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -2655,8 +2887,10 @@
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -2666,8 +2900,10 @@
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+    </row>
+    <row r="100" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -2677,8 +2913,10 @@
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+    </row>
+    <row r="101" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -2688,8 +2926,10 @@
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -2699,8 +2939,10 @@
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -2710,8 +2952,10 @@
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+    </row>
+    <row r="104" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -2721,8 +2965,10 @@
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -2732,8 +2978,10 @@
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -2743,8 +2991,10 @@
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+    </row>
+    <row r="107" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -2754,8 +3004,10 @@
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -2765,8 +3017,10 @@
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+    </row>
+    <row r="109" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -2776,8 +3030,10 @@
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+    </row>
+    <row r="110" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="9"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -2787,8 +3043,10 @@
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+    </row>
+    <row r="111" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="9"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -2798,8 +3056,10 @@
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+    </row>
+    <row r="112" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
@@ -2809,8 +3069,10 @@
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+    </row>
+    <row r="113" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="9"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -2820,8 +3082,10 @@
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+    </row>
+    <row r="114" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="9"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
@@ -2831,8 +3095,10 @@
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+    </row>
+    <row r="115" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="9"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -2842,8 +3108,10 @@
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+    </row>
+    <row r="116" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -2853,8 +3121,10 @@
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+    </row>
+    <row r="117" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -2864,8 +3134,10 @@
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+    </row>
+    <row r="118" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="9"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
@@ -2875,8 +3147,10 @@
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
+    </row>
+    <row r="119" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="9"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -2886,8 +3160,10 @@
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+    </row>
+    <row r="120" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
@@ -2897,8 +3173,10 @@
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J120" s="7"/>
+      <c r="K120" s="7"/>
+    </row>
+    <row r="121" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -2908,8 +3186,10 @@
       <c r="G121" s="7"/>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+    </row>
+    <row r="122" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="9"/>
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
@@ -2919,8 +3199,10 @@
       <c r="G122" s="7"/>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+    </row>
+    <row r="123" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
@@ -2930,8 +3212,10 @@
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+    </row>
+    <row r="124" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="9"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
@@ -2941,8 +3225,10 @@
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J124" s="7"/>
+      <c r="K124" s="7"/>
+    </row>
+    <row r="125" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="9"/>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
@@ -2952,8 +3238,10 @@
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+    </row>
+    <row r="126" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="9"/>
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
@@ -2963,8 +3251,10 @@
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J126" s="7"/>
+      <c r="K126" s="7"/>
+    </row>
+    <row r="127" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="9"/>
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
@@ -2974,8 +3264,10 @@
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+    </row>
+    <row r="128" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9"/>
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
@@ -2985,8 +3277,10 @@
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J128" s="7"/>
+      <c r="K128" s="7"/>
+    </row>
+    <row r="129" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -2996,8 +3290,10 @@
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+    </row>
+    <row r="130" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="9"/>
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
@@ -3007,8 +3303,10 @@
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J130" s="7"/>
+      <c r="K130" s="7"/>
+    </row>
+    <row r="131" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="9"/>
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
@@ -3018,8 +3316,10 @@
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+    </row>
+    <row r="132" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="9"/>
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
@@ -3029,8 +3329,10 @@
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J132" s="7"/>
+      <c r="K132" s="7"/>
+    </row>
+    <row r="133" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="9"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -3040,8 +3342,10 @@
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+    </row>
+    <row r="134" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="9"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -3051,8 +3355,10 @@
       <c r="G134" s="7"/>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
-    </row>
-    <row r="135" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+    </row>
+    <row r="135" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="9"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -3062,8 +3368,10 @@
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
-    </row>
-    <row r="136" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+    </row>
+    <row r="136" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="9"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
@@ -3073,8 +3381,10 @@
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
-    </row>
-    <row r="137" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J136" s="7"/>
+      <c r="K136" s="7"/>
+    </row>
+    <row r="137" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="9"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -3084,8 +3394,10 @@
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
-    </row>
-    <row r="138" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+    </row>
+    <row r="138" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="9"/>
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
@@ -3095,8 +3407,10 @@
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
-    </row>
-    <row r="139" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J138" s="7"/>
+      <c r="K138" s="7"/>
+    </row>
+    <row r="139" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="9"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -3106,8 +3420,10 @@
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
-    </row>
-    <row r="140" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+    </row>
+    <row r="140" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="9"/>
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
@@ -3117,8 +3433,10 @@
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
-    </row>
-    <row r="141" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J140" s="7"/>
+      <c r="K140" s="7"/>
+    </row>
+    <row r="141" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="9"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -3128,8 +3446,10 @@
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
-    </row>
-    <row r="142" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+    </row>
+    <row r="142" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
@@ -3139,8 +3459,10 @@
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
-    </row>
-    <row r="143" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J142" s="7"/>
+      <c r="K142" s="7"/>
+    </row>
+    <row r="143" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
@@ -3150,8 +3472,10 @@
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
-    </row>
-    <row r="144" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+    </row>
+    <row r="144" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
@@ -3161,8 +3485,10 @@
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
-    </row>
-    <row r="145" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J144" s="7"/>
+      <c r="K144" s="7"/>
+    </row>
+    <row r="145" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
@@ -3172,8 +3498,10 @@
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
-    </row>
-    <row r="146" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+    </row>
+    <row r="146" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
@@ -3183,8 +3511,10 @@
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
-    </row>
-    <row r="147" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J146" s="7"/>
+      <c r="K146" s="7"/>
+    </row>
+    <row r="147" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
@@ -3194,8 +3524,10 @@
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
-    </row>
-    <row r="148" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+    </row>
+    <row r="148" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
@@ -3205,8 +3537,10 @@
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
-    </row>
-    <row r="149" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J148" s="7"/>
+      <c r="K148" s="7"/>
+    </row>
+    <row r="149" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -3216,8 +3550,10 @@
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
-    </row>
-    <row r="150" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J149" s="7"/>
+      <c r="K149" s="7"/>
+    </row>
+    <row r="150" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
@@ -3227,8 +3563,10 @@
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
-    </row>
-    <row r="151" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J150" s="7"/>
+      <c r="K150" s="7"/>
+    </row>
+    <row r="151" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
@@ -3238,8 +3576,10 @@
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
-    </row>
-    <row r="152" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J151" s="7"/>
+      <c r="K151" s="7"/>
+    </row>
+    <row r="152" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="9"/>
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
@@ -3249,8 +3589,10 @@
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
-    </row>
-    <row r="153" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J152" s="7"/>
+      <c r="K152" s="7"/>
+    </row>
+    <row r="153" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="9"/>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -3260,8 +3602,10 @@
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
-    </row>
-    <row r="154" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+    </row>
+    <row r="154" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9"/>
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
@@ -3271,8 +3615,10 @@
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
-    </row>
-    <row r="155" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J154" s="7"/>
+      <c r="K154" s="7"/>
+    </row>
+    <row r="155" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="9"/>
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
@@ -3282,8 +3628,10 @@
       <c r="G155" s="7"/>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
-    </row>
-    <row r="156" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
+    </row>
+    <row r="156" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="9"/>
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
@@ -3293,8 +3641,10 @@
       <c r="G156" s="7"/>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
-    </row>
-    <row r="157" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J156" s="7"/>
+      <c r="K156" s="7"/>
+    </row>
+    <row r="157" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="9"/>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -3304,8 +3654,10 @@
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-    </row>
-    <row r="158" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J157" s="7"/>
+      <c r="K157" s="7"/>
+    </row>
+    <row r="158" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
@@ -3315,8 +3667,10 @@
       <c r="G158" s="7"/>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-    </row>
-    <row r="159" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J158" s="7"/>
+      <c r="K158" s="7"/>
+    </row>
+    <row r="159" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="9"/>
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
@@ -3326,8 +3680,10 @@
       <c r="G159" s="7"/>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
-    </row>
-    <row r="160" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J159" s="7"/>
+      <c r="K159" s="7"/>
+    </row>
+    <row r="160" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="9"/>
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
@@ -3337,8 +3693,10 @@
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
-    </row>
-    <row r="161" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J160" s="7"/>
+      <c r="K160" s="7"/>
+    </row>
+    <row r="161" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="9"/>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
@@ -3348,8 +3706,10 @@
       <c r="G161" s="7"/>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
-    </row>
-    <row r="162" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J161" s="7"/>
+      <c r="K161" s="7"/>
+    </row>
+    <row r="162" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="9"/>
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
@@ -3359,8 +3719,10 @@
       <c r="G162" s="7"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
-    </row>
-    <row r="163" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J162" s="7"/>
+      <c r="K162" s="7"/>
+    </row>
+    <row r="163" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="9"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
@@ -3370,8 +3732,10 @@
       <c r="G163" s="7"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
-    </row>
-    <row r="164" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J163" s="7"/>
+      <c r="K163" s="7"/>
+    </row>
+    <row r="164" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="9"/>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
@@ -3381,8 +3745,10 @@
       <c r="G164" s="7"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
-    </row>
-    <row r="165" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J164" s="7"/>
+      <c r="K164" s="7"/>
+    </row>
+    <row r="165" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="9"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -3392,8 +3758,10 @@
       <c r="G165" s="7"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
-    </row>
-    <row r="166" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J165" s="7"/>
+      <c r="K165" s="7"/>
+    </row>
+    <row r="166" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="9"/>
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
@@ -3403,8 +3771,10 @@
       <c r="G166" s="7"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
-    </row>
-    <row r="167" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J166" s="7"/>
+      <c r="K166" s="7"/>
+    </row>
+    <row r="167" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="9"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
@@ -3414,8 +3784,10 @@
       <c r="G167" s="7"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
-    </row>
-    <row r="168" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J167" s="7"/>
+      <c r="K167" s="7"/>
+    </row>
+    <row r="168" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="9"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
@@ -3425,8 +3797,10 @@
       <c r="G168" s="7"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
-    </row>
-    <row r="169" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J168" s="7"/>
+      <c r="K168" s="7"/>
+    </row>
+    <row r="169" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="9"/>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -3436,8 +3810,10 @@
       <c r="G169" s="7"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
-    </row>
-    <row r="170" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J169" s="7"/>
+      <c r="K169" s="7"/>
+    </row>
+    <row r="170" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="9"/>
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
@@ -3447,8 +3823,10 @@
       <c r="G170" s="7"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
-    </row>
-    <row r="171" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J170" s="7"/>
+      <c r="K170" s="7"/>
+    </row>
+    <row r="171" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="9"/>
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
@@ -3458,8 +3836,10 @@
       <c r="G171" s="7"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
-    </row>
-    <row r="172" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J171" s="7"/>
+      <c r="K171" s="7"/>
+    </row>
+    <row r="172" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="9"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -3469,8 +3849,10 @@
       <c r="G172" s="7"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-    </row>
-    <row r="173" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J172" s="7"/>
+      <c r="K172" s="7"/>
+    </row>
+    <row r="173" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="9"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -3480,8 +3862,10 @@
       <c r="G173" s="7"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
-    </row>
-    <row r="174" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J173" s="7"/>
+      <c r="K173" s="7"/>
+    </row>
+    <row r="174" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="9"/>
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
@@ -3491,8 +3875,10 @@
       <c r="G174" s="7"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
-    </row>
-    <row r="175" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J174" s="7"/>
+      <c r="K174" s="7"/>
+    </row>
+    <row r="175" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="9"/>
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
@@ -3502,8 +3888,10 @@
       <c r="G175" s="7"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
-    </row>
-    <row r="176" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J175" s="7"/>
+      <c r="K175" s="7"/>
+    </row>
+    <row r="176" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="9"/>
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
@@ -3513,8 +3901,10 @@
       <c r="G176" s="7"/>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
-    </row>
-    <row r="177" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J176" s="7"/>
+      <c r="K176" s="7"/>
+    </row>
+    <row r="177" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="9"/>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
@@ -3524,8 +3914,10 @@
       <c r="G177" s="7"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
-    </row>
-    <row r="178" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J177" s="7"/>
+      <c r="K177" s="7"/>
+    </row>
+    <row r="178" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="9"/>
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
@@ -3535,8 +3927,10 @@
       <c r="G178" s="7"/>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
-    </row>
-    <row r="179" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J178" s="7"/>
+      <c r="K178" s="7"/>
+    </row>
+    <row r="179" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="9"/>
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
@@ -3546,8 +3940,10 @@
       <c r="G179" s="7"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
-    </row>
-    <row r="180" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J179" s="7"/>
+      <c r="K179" s="7"/>
+    </row>
+    <row r="180" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9"/>
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
@@ -3557,8 +3953,10 @@
       <c r="G180" s="7"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
-    </row>
-    <row r="181" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J180" s="7"/>
+      <c r="K180" s="7"/>
+    </row>
+    <row r="181" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="9"/>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
@@ -3568,8 +3966,10 @@
       <c r="G181" s="7"/>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
-    </row>
-    <row r="182" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J181" s="7"/>
+      <c r="K181" s="7"/>
+    </row>
+    <row r="182" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="9"/>
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
@@ -3579,8 +3979,10 @@
       <c r="G182" s="7"/>
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
-    </row>
-    <row r="183" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J182" s="7"/>
+      <c r="K182" s="7"/>
+    </row>
+    <row r="183" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="9"/>
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
@@ -3590,8 +3992,10 @@
       <c r="G183" s="7"/>
       <c r="H183" s="7"/>
       <c r="I183" s="7"/>
-    </row>
-    <row r="184" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J183" s="7"/>
+      <c r="K183" s="7"/>
+    </row>
+    <row r="184" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="9"/>
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
@@ -3601,8 +4005,10 @@
       <c r="G184" s="7"/>
       <c r="H184" s="7"/>
       <c r="I184" s="7"/>
-    </row>
-    <row r="185" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J184" s="7"/>
+      <c r="K184" s="7"/>
+    </row>
+    <row r="185" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="9"/>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
@@ -3612,8 +4018,10 @@
       <c r="G185" s="7"/>
       <c r="H185" s="7"/>
       <c r="I185" s="7"/>
-    </row>
-    <row r="186" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J185" s="7"/>
+      <c r="K185" s="7"/>
+    </row>
+    <row r="186" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="9"/>
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
@@ -3623,8 +4031,10 @@
       <c r="G186" s="7"/>
       <c r="H186" s="7"/>
       <c r="I186" s="7"/>
-    </row>
-    <row r="187" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J186" s="7"/>
+      <c r="K186" s="7"/>
+    </row>
+    <row r="187" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="9"/>
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
@@ -3634,8 +4044,10 @@
       <c r="G187" s="7"/>
       <c r="H187" s="7"/>
       <c r="I187" s="7"/>
-    </row>
-    <row r="188" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+    </row>
+    <row r="188" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="9"/>
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
@@ -3645,8 +4057,10 @@
       <c r="G188" s="7"/>
       <c r="H188" s="7"/>
       <c r="I188" s="7"/>
-    </row>
-    <row r="189" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J188" s="7"/>
+      <c r="K188" s="7"/>
+    </row>
+    <row r="189" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="9"/>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
@@ -3656,8 +4070,10 @@
       <c r="G189" s="7"/>
       <c r="H189" s="7"/>
       <c r="I189" s="7"/>
-    </row>
-    <row r="190" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J189" s="7"/>
+      <c r="K189" s="7"/>
+    </row>
+    <row r="190" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="9"/>
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
@@ -3667,8 +4083,10 @@
       <c r="G190" s="7"/>
       <c r="H190" s="7"/>
       <c r="I190" s="7"/>
-    </row>
-    <row r="191" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J190" s="7"/>
+      <c r="K190" s="7"/>
+    </row>
+    <row r="191" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="9"/>
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
@@ -3678,8 +4096,10 @@
       <c r="G191" s="7"/>
       <c r="H191" s="7"/>
       <c r="I191" s="7"/>
-    </row>
-    <row r="192" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J191" s="7"/>
+      <c r="K191" s="7"/>
+    </row>
+    <row r="192" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="9"/>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
@@ -3689,8 +4109,10 @@
       <c r="G192" s="7"/>
       <c r="H192" s="7"/>
       <c r="I192" s="7"/>
-    </row>
-    <row r="193" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+    </row>
+    <row r="193" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="9"/>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
@@ -3700,8 +4122,10 @@
       <c r="G193" s="7"/>
       <c r="H193" s="7"/>
       <c r="I193" s="7"/>
-    </row>
-    <row r="194" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J193" s="7"/>
+      <c r="K193" s="7"/>
+    </row>
+    <row r="194" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="9"/>
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
@@ -3711,8 +4135,10 @@
       <c r="G194" s="7"/>
       <c r="H194" s="7"/>
       <c r="I194" s="7"/>
-    </row>
-    <row r="195" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J194" s="7"/>
+      <c r="K194" s="7"/>
+    </row>
+    <row r="195" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="9"/>
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
@@ -3722,8 +4148,10 @@
       <c r="G195" s="7"/>
       <c r="H195" s="7"/>
       <c r="I195" s="7"/>
-    </row>
-    <row r="196" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J195" s="7"/>
+      <c r="K195" s="7"/>
+    </row>
+    <row r="196" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="9"/>
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
@@ -3733,8 +4161,10 @@
       <c r="G196" s="7"/>
       <c r="H196" s="7"/>
       <c r="I196" s="7"/>
-    </row>
-    <row r="197" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J196" s="7"/>
+      <c r="K196" s="7"/>
+    </row>
+    <row r="197" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="9"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -3744,8 +4174,10 @@
       <c r="G197" s="7"/>
       <c r="H197" s="7"/>
       <c r="I197" s="7"/>
-    </row>
-    <row r="198" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J197" s="7"/>
+      <c r="K197" s="7"/>
+    </row>
+    <row r="198" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="9"/>
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
@@ -3755,8 +4187,10 @@
       <c r="G198" s="7"/>
       <c r="H198" s="7"/>
       <c r="I198" s="7"/>
-    </row>
-    <row r="199" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J198" s="7"/>
+      <c r="K198" s="7"/>
+    </row>
+    <row r="199" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="9"/>
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
@@ -3766,8 +4200,10 @@
       <c r="G199" s="7"/>
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
-    </row>
-    <row r="200" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J199" s="7"/>
+      <c r="K199" s="7"/>
+    </row>
+    <row r="200" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
@@ -3777,8 +4213,10 @@
       <c r="G200" s="7"/>
       <c r="H200" s="7"/>
       <c r="I200" s="7"/>
-    </row>
-    <row r="201" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J200" s="7"/>
+      <c r="K200" s="7"/>
+    </row>
+    <row r="201" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
@@ -3788,8 +4226,10 @@
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
       <c r="I201" s="7"/>
-    </row>
-    <row r="202" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J201" s="7"/>
+      <c r="K201" s="7"/>
+    </row>
+    <row r="202" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="9"/>
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
@@ -3799,8 +4239,10 @@
       <c r="G202" s="7"/>
       <c r="H202" s="7"/>
       <c r="I202" s="7"/>
-    </row>
-    <row r="203" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J202" s="7"/>
+      <c r="K202" s="7"/>
+    </row>
+    <row r="203" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="9"/>
       <c r="B203" s="9"/>
       <c r="C203" s="9"/>
@@ -3810,8 +4252,10 @@
       <c r="G203" s="7"/>
       <c r="H203" s="7"/>
       <c r="I203" s="7"/>
-    </row>
-    <row r="204" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J203" s="7"/>
+      <c r="K203" s="7"/>
+    </row>
+    <row r="204" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="9"/>
       <c r="B204" s="9"/>
       <c r="C204" s="9"/>
@@ -3821,8 +4265,10 @@
       <c r="G204" s="7"/>
       <c r="H204" s="7"/>
       <c r="I204" s="7"/>
-    </row>
-    <row r="205" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J204" s="7"/>
+      <c r="K204" s="7"/>
+    </row>
+    <row r="205" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="9"/>
       <c r="B205" s="9"/>
       <c r="C205" s="9"/>
@@ -3832,8 +4278,10 @@
       <c r="G205" s="7"/>
       <c r="H205" s="7"/>
       <c r="I205" s="7"/>
-    </row>
-    <row r="206" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+    </row>
+    <row r="206" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="9"/>
       <c r="B206" s="9"/>
       <c r="C206" s="9"/>
@@ -3843,8 +4291,10 @@
       <c r="G206" s="7"/>
       <c r="H206" s="7"/>
       <c r="I206" s="7"/>
-    </row>
-    <row r="207" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J206" s="7"/>
+      <c r="K206" s="7"/>
+    </row>
+    <row r="207" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="9"/>
       <c r="B207" s="9"/>
       <c r="C207" s="9"/>
@@ -3854,8 +4304,10 @@
       <c r="G207" s="7"/>
       <c r="H207" s="7"/>
       <c r="I207" s="7"/>
-    </row>
-    <row r="208" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J207" s="7"/>
+      <c r="K207" s="7"/>
+    </row>
+    <row r="208" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="9"/>
       <c r="B208" s="9"/>
       <c r="C208" s="9"/>
@@ -3865,8 +4317,10 @@
       <c r="G208" s="7"/>
       <c r="H208" s="7"/>
       <c r="I208" s="7"/>
-    </row>
-    <row r="209" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J208" s="7"/>
+      <c r="K208" s="7"/>
+    </row>
+    <row r="209" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="9"/>
       <c r="B209" s="9"/>
       <c r="C209" s="9"/>
@@ -3876,8 +4330,10 @@
       <c r="G209" s="7"/>
       <c r="H209" s="7"/>
       <c r="I209" s="7"/>
-    </row>
-    <row r="210" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J209" s="7"/>
+      <c r="K209" s="7"/>
+    </row>
+    <row r="210" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="9"/>
       <c r="B210" s="9"/>
       <c r="C210" s="9"/>
@@ -3887,8 +4343,10 @@
       <c r="G210" s="7"/>
       <c r="H210" s="7"/>
       <c r="I210" s="7"/>
-    </row>
-    <row r="211" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J210" s="7"/>
+      <c r="K210" s="7"/>
+    </row>
+    <row r="211" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="9"/>
       <c r="B211" s="9"/>
       <c r="C211" s="9"/>
@@ -3898,8 +4356,10 @@
       <c r="G211" s="7"/>
       <c r="H211" s="7"/>
       <c r="I211" s="7"/>
-    </row>
-    <row r="212" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J211" s="7"/>
+      <c r="K211" s="7"/>
+    </row>
+    <row r="212" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="9"/>
       <c r="B212" s="9"/>
       <c r="C212" s="9"/>
@@ -3909,8 +4369,10 @@
       <c r="G212" s="7"/>
       <c r="H212" s="7"/>
       <c r="I212" s="7"/>
-    </row>
-    <row r="213" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J212" s="7"/>
+      <c r="K212" s="7"/>
+    </row>
+    <row r="213" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="9"/>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
@@ -3920,8 +4382,10 @@
       <c r="G213" s="7"/>
       <c r="H213" s="7"/>
       <c r="I213" s="7"/>
-    </row>
-    <row r="214" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J213" s="7"/>
+      <c r="K213" s="7"/>
+    </row>
+    <row r="214" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="9"/>
       <c r="B214" s="9"/>
       <c r="C214" s="9"/>
@@ -3931,8 +4395,10 @@
       <c r="G214" s="7"/>
       <c r="H214" s="7"/>
       <c r="I214" s="7"/>
-    </row>
-    <row r="215" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J214" s="7"/>
+      <c r="K214" s="7"/>
+    </row>
+    <row r="215" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="9"/>
       <c r="B215" s="9"/>
       <c r="C215" s="9"/>
@@ -3942,8 +4408,10 @@
       <c r="G215" s="7"/>
       <c r="H215" s="7"/>
       <c r="I215" s="7"/>
-    </row>
-    <row r="216" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J215" s="7"/>
+      <c r="K215" s="7"/>
+    </row>
+    <row r="216" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="9"/>
       <c r="B216" s="9"/>
       <c r="C216" s="9"/>
@@ -3953,8 +4421,10 @@
       <c r="G216" s="7"/>
       <c r="H216" s="7"/>
       <c r="I216" s="7"/>
-    </row>
-    <row r="217" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J216" s="7"/>
+      <c r="K216" s="7"/>
+    </row>
+    <row r="217" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="9"/>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
@@ -3964,8 +4434,10 @@
       <c r="G217" s="7"/>
       <c r="H217" s="7"/>
       <c r="I217" s="7"/>
-    </row>
-    <row r="218" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J217" s="7"/>
+      <c r="K217" s="7"/>
+    </row>
+    <row r="218" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="9"/>
       <c r="B218" s="9"/>
       <c r="C218" s="9"/>
@@ -3975,8 +4447,10 @@
       <c r="G218" s="7"/>
       <c r="H218" s="7"/>
       <c r="I218" s="7"/>
-    </row>
-    <row r="219" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J218" s="7"/>
+      <c r="K218" s="7"/>
+    </row>
+    <row r="219" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="9"/>
       <c r="B219" s="9"/>
       <c r="C219" s="9"/>
@@ -3986,8 +4460,10 @@
       <c r="G219" s="7"/>
       <c r="H219" s="7"/>
       <c r="I219" s="7"/>
-    </row>
-    <row r="220" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J219" s="7"/>
+      <c r="K219" s="7"/>
+    </row>
+    <row r="220" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="9"/>
       <c r="B220" s="9"/>
       <c r="C220" s="9"/>
@@ -3997,8 +4473,10 @@
       <c r="G220" s="7"/>
       <c r="H220" s="7"/>
       <c r="I220" s="7"/>
-    </row>
-    <row r="221" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J220" s="7"/>
+      <c r="K220" s="7"/>
+    </row>
+    <row r="221" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="9"/>
       <c r="B221" s="9"/>
       <c r="C221" s="9"/>
@@ -4008,8 +4486,10 @@
       <c r="G221" s="7"/>
       <c r="H221" s="7"/>
       <c r="I221" s="7"/>
-    </row>
-    <row r="222" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J221" s="7"/>
+      <c r="K221" s="7"/>
+    </row>
+    <row r="222" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="9"/>
       <c r="B222" s="9"/>
       <c r="C222" s="9"/>
@@ -4019,8 +4499,10 @@
       <c r="G222" s="7"/>
       <c r="H222" s="7"/>
       <c r="I222" s="7"/>
-    </row>
-    <row r="223" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J222" s="7"/>
+      <c r="K222" s="7"/>
+    </row>
+    <row r="223" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="9"/>
       <c r="B223" s="9"/>
       <c r="C223" s="9"/>
@@ -4030,8 +4512,10 @@
       <c r="G223" s="7"/>
       <c r="H223" s="7"/>
       <c r="I223" s="7"/>
-    </row>
-    <row r="224" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J223" s="7"/>
+      <c r="K223" s="7"/>
+    </row>
+    <row r="224" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="B224" s="9"/>
       <c r="C224" s="9"/>
@@ -4041,8 +4525,10 @@
       <c r="G224" s="7"/>
       <c r="H224" s="7"/>
       <c r="I224" s="7"/>
-    </row>
-    <row r="225" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J224" s="7"/>
+      <c r="K224" s="7"/>
+    </row>
+    <row r="225" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="9"/>
       <c r="B225" s="9"/>
       <c r="C225" s="9"/>
@@ -4052,8 +4538,10 @@
       <c r="G225" s="7"/>
       <c r="H225" s="7"/>
       <c r="I225" s="7"/>
-    </row>
-    <row r="226" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J225" s="7"/>
+      <c r="K225" s="7"/>
+    </row>
+    <row r="226" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="9"/>
       <c r="B226" s="9"/>
       <c r="C226" s="9"/>
@@ -4063,8 +4551,10 @@
       <c r="G226" s="7"/>
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
-    </row>
-    <row r="227" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J226" s="7"/>
+      <c r="K226" s="7"/>
+    </row>
+    <row r="227" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="9"/>
       <c r="B227" s="9"/>
       <c r="C227" s="9"/>
@@ -4074,8 +4564,10 @@
       <c r="G227" s="7"/>
       <c r="H227" s="7"/>
       <c r="I227" s="7"/>
-    </row>
-    <row r="228" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J227" s="7"/>
+      <c r="K227" s="7"/>
+    </row>
+    <row r="228" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="9"/>
       <c r="B228" s="9"/>
       <c r="C228" s="9"/>
@@ -4085,8 +4577,10 @@
       <c r="G228" s="7"/>
       <c r="H228" s="7"/>
       <c r="I228" s="7"/>
-    </row>
-    <row r="229" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J228" s="7"/>
+      <c r="K228" s="7"/>
+    </row>
+    <row r="229" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="9"/>
       <c r="B229" s="9"/>
       <c r="C229" s="9"/>
@@ -4096,8 +4590,10 @@
       <c r="G229" s="7"/>
       <c r="H229" s="7"/>
       <c r="I229" s="7"/>
-    </row>
-    <row r="230" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J229" s="7"/>
+      <c r="K229" s="7"/>
+    </row>
+    <row r="230" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="9"/>
       <c r="B230" s="9"/>
       <c r="C230" s="9"/>
@@ -4107,8 +4603,10 @@
       <c r="G230" s="7"/>
       <c r="H230" s="7"/>
       <c r="I230" s="7"/>
-    </row>
-    <row r="231" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J230" s="7"/>
+      <c r="K230" s="7"/>
+    </row>
+    <row r="231" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="9"/>
       <c r="B231" s="9"/>
       <c r="C231" s="9"/>
@@ -4118,8 +4616,10 @@
       <c r="G231" s="7"/>
       <c r="H231" s="7"/>
       <c r="I231" s="7"/>
-    </row>
-    <row r="232" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J231" s="7"/>
+      <c r="K231" s="7"/>
+    </row>
+    <row r="232" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="9"/>
       <c r="B232" s="9"/>
       <c r="C232" s="9"/>
@@ -4129,8 +4629,10 @@
       <c r="G232" s="7"/>
       <c r="H232" s="7"/>
       <c r="I232" s="7"/>
-    </row>
-    <row r="233" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J232" s="7"/>
+      <c r="K232" s="7"/>
+    </row>
+    <row r="233" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="9"/>
       <c r="B233" s="9"/>
       <c r="C233" s="9"/>
@@ -4140,8 +4642,10 @@
       <c r="G233" s="7"/>
       <c r="H233" s="7"/>
       <c r="I233" s="7"/>
-    </row>
-    <row r="234" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J233" s="7"/>
+      <c r="K233" s="7"/>
+    </row>
+    <row r="234" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="9"/>
       <c r="B234" s="9"/>
       <c r="C234" s="9"/>
@@ -4151,8 +4655,10 @@
       <c r="G234" s="7"/>
       <c r="H234" s="7"/>
       <c r="I234" s="7"/>
-    </row>
-    <row r="235" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J234" s="7"/>
+      <c r="K234" s="7"/>
+    </row>
+    <row r="235" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="9"/>
       <c r="B235" s="9"/>
       <c r="C235" s="9"/>
@@ -4162,8 +4668,10 @@
       <c r="G235" s="7"/>
       <c r="H235" s="7"/>
       <c r="I235" s="7"/>
-    </row>
-    <row r="236" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J235" s="7"/>
+      <c r="K235" s="7"/>
+    </row>
+    <row r="236" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="9"/>
       <c r="B236" s="9"/>
       <c r="C236" s="9"/>
@@ -4173,8 +4681,10 @@
       <c r="G236" s="7"/>
       <c r="H236" s="7"/>
       <c r="I236" s="7"/>
-    </row>
-    <row r="237" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J236" s="7"/>
+      <c r="K236" s="7"/>
+    </row>
+    <row r="237" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="9"/>
       <c r="B237" s="9"/>
       <c r="C237" s="9"/>
@@ -4184,8 +4694,10 @@
       <c r="G237" s="7"/>
       <c r="H237" s="7"/>
       <c r="I237" s="7"/>
-    </row>
-    <row r="238" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J237" s="7"/>
+      <c r="K237" s="7"/>
+    </row>
+    <row r="238" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="9"/>
       <c r="B238" s="9"/>
       <c r="C238" s="9"/>
@@ -4195,8 +4707,10 @@
       <c r="G238" s="7"/>
       <c r="H238" s="7"/>
       <c r="I238" s="7"/>
-    </row>
-    <row r="239" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J238" s="7"/>
+      <c r="K238" s="7"/>
+    </row>
+    <row r="239" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="9"/>
       <c r="B239" s="9"/>
       <c r="C239" s="9"/>
@@ -4206,8 +4720,10 @@
       <c r="G239" s="7"/>
       <c r="H239" s="7"/>
       <c r="I239" s="7"/>
-    </row>
-    <row r="240" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J239" s="7"/>
+      <c r="K239" s="7"/>
+    </row>
+    <row r="240" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="9"/>
       <c r="B240" s="9"/>
       <c r="C240" s="9"/>
@@ -4217,8 +4733,10 @@
       <c r="G240" s="7"/>
       <c r="H240" s="7"/>
       <c r="I240" s="7"/>
-    </row>
-    <row r="241" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J240" s="7"/>
+      <c r="K240" s="7"/>
+    </row>
+    <row r="241" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="9"/>
       <c r="B241" s="9"/>
       <c r="C241" s="9"/>
@@ -4228,8 +4746,10 @@
       <c r="G241" s="7"/>
       <c r="H241" s="7"/>
       <c r="I241" s="7"/>
-    </row>
-    <row r="242" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J241" s="7"/>
+      <c r="K241" s="7"/>
+    </row>
+    <row r="242" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="9"/>
       <c r="B242" s="9"/>
       <c r="C242" s="9"/>
@@ -4239,8 +4759,10 @@
       <c r="G242" s="7"/>
       <c r="H242" s="7"/>
       <c r="I242" s="7"/>
-    </row>
-    <row r="243" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J242" s="7"/>
+      <c r="K242" s="7"/>
+    </row>
+    <row r="243" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="9"/>
       <c r="B243" s="9"/>
       <c r="C243" s="9"/>
@@ -4250,8 +4772,10 @@
       <c r="G243" s="7"/>
       <c r="H243" s="7"/>
       <c r="I243" s="7"/>
-    </row>
-    <row r="244" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J243" s="7"/>
+      <c r="K243" s="7"/>
+    </row>
+    <row r="244" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="9"/>
       <c r="B244" s="9"/>
       <c r="C244" s="9"/>
@@ -4261,8 +4785,10 @@
       <c r="G244" s="7"/>
       <c r="H244" s="7"/>
       <c r="I244" s="7"/>
-    </row>
-    <row r="245" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J244" s="7"/>
+      <c r="K244" s="7"/>
+    </row>
+    <row r="245" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="9"/>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
@@ -4272,8 +4798,10 @@
       <c r="G245" s="7"/>
       <c r="H245" s="7"/>
       <c r="I245" s="7"/>
-    </row>
-    <row r="246" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J245" s="7"/>
+      <c r="K245" s="7"/>
+    </row>
+    <row r="246" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="9"/>
       <c r="B246" s="9"/>
       <c r="C246" s="9"/>
@@ -4283,8 +4811,10 @@
       <c r="G246" s="7"/>
       <c r="H246" s="7"/>
       <c r="I246" s="7"/>
-    </row>
-    <row r="247" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J246" s="7"/>
+      <c r="K246" s="7"/>
+    </row>
+    <row r="247" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="9"/>
       <c r="B247" s="9"/>
       <c r="C247" s="9"/>
@@ -4294,8 +4824,10 @@
       <c r="G247" s="7"/>
       <c r="H247" s="7"/>
       <c r="I247" s="7"/>
-    </row>
-    <row r="248" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J247" s="7"/>
+      <c r="K247" s="7"/>
+    </row>
+    <row r="248" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="9"/>
       <c r="B248" s="9"/>
       <c r="C248" s="9"/>
@@ -4305,8 +4837,10 @@
       <c r="G248" s="7"/>
       <c r="H248" s="7"/>
       <c r="I248" s="7"/>
-    </row>
-    <row r="249" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J248" s="7"/>
+      <c r="K248" s="7"/>
+    </row>
+    <row r="249" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="9"/>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
@@ -4316,8 +4850,10 @@
       <c r="G249" s="7"/>
       <c r="H249" s="7"/>
       <c r="I249" s="7"/>
-    </row>
-    <row r="250" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J249" s="7"/>
+      <c r="K249" s="7"/>
+    </row>
+    <row r="250" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="9"/>
       <c r="B250" s="9"/>
       <c r="C250" s="9"/>
@@ -4327,8 +4863,10 @@
       <c r="G250" s="7"/>
       <c r="H250" s="7"/>
       <c r="I250" s="7"/>
-    </row>
-    <row r="251" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J250" s="7"/>
+      <c r="K250" s="7"/>
+    </row>
+    <row r="251" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="9"/>
       <c r="B251" s="9"/>
       <c r="C251" s="9"/>
@@ -4338,8 +4876,10 @@
       <c r="G251" s="7"/>
       <c r="H251" s="7"/>
       <c r="I251" s="7"/>
-    </row>
-    <row r="252" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J251" s="7"/>
+      <c r="K251" s="7"/>
+    </row>
+    <row r="252" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="9"/>
       <c r="B252" s="9"/>
       <c r="C252" s="9"/>
@@ -4349,8 +4889,10 @@
       <c r="G252" s="7"/>
       <c r="H252" s="7"/>
       <c r="I252" s="7"/>
-    </row>
-    <row r="253" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J252" s="7"/>
+      <c r="K252" s="7"/>
+    </row>
+    <row r="253" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="9"/>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
@@ -4360,8 +4902,10 @@
       <c r="G253" s="7"/>
       <c r="H253" s="7"/>
       <c r="I253" s="7"/>
-    </row>
-    <row r="254" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J253" s="7"/>
+      <c r="K253" s="7"/>
+    </row>
+    <row r="254" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="9"/>
       <c r="B254" s="9"/>
       <c r="C254" s="9"/>
@@ -4371,8 +4915,10 @@
       <c r="G254" s="7"/>
       <c r="H254" s="7"/>
       <c r="I254" s="7"/>
-    </row>
-    <row r="255" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J254" s="7"/>
+      <c r="K254" s="7"/>
+    </row>
+    <row r="255" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="9"/>
       <c r="B255" s="9"/>
       <c r="C255" s="9"/>
@@ -4382,8 +4928,10 @@
       <c r="G255" s="7"/>
       <c r="H255" s="7"/>
       <c r="I255" s="7"/>
-    </row>
-    <row r="256" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J255" s="7"/>
+      <c r="K255" s="7"/>
+    </row>
+    <row r="256" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="9"/>
       <c r="B256" s="9"/>
       <c r="C256" s="9"/>
@@ -4393,8 +4941,10 @@
       <c r="G256" s="7"/>
       <c r="H256" s="7"/>
       <c r="I256" s="7"/>
-    </row>
-    <row r="257" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J256" s="7"/>
+      <c r="K256" s="7"/>
+    </row>
+    <row r="257" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="9"/>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -4404,8 +4954,10 @@
       <c r="G257" s="7"/>
       <c r="H257" s="7"/>
       <c r="I257" s="7"/>
-    </row>
-    <row r="258" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J257" s="7"/>
+      <c r="K257" s="7"/>
+    </row>
+    <row r="258" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="9"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
@@ -4415,8 +4967,10 @@
       <c r="G258" s="7"/>
       <c r="H258" s="7"/>
       <c r="I258" s="7"/>
-    </row>
-    <row r="259" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J258" s="7"/>
+      <c r="K258" s="7"/>
+    </row>
+    <row r="259" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="9"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
@@ -4426,8 +4980,10 @@
       <c r="G259" s="7"/>
       <c r="H259" s="7"/>
       <c r="I259" s="7"/>
-    </row>
-    <row r="260" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J259" s="7"/>
+      <c r="K259" s="7"/>
+    </row>
+    <row r="260" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="9"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
@@ -4437,8 +4993,10 @@
       <c r="G260" s="7"/>
       <c r="H260" s="7"/>
       <c r="I260" s="7"/>
-    </row>
-    <row r="261" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J260" s="7"/>
+      <c r="K260" s="7"/>
+    </row>
+    <row r="261" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="9"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
@@ -4448,8 +5006,10 @@
       <c r="G261" s="7"/>
       <c r="H261" s="7"/>
       <c r="I261" s="7"/>
-    </row>
-    <row r="262" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J261" s="7"/>
+      <c r="K261" s="7"/>
+    </row>
+    <row r="262" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="9"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
@@ -4459,8 +5019,10 @@
       <c r="G262" s="7"/>
       <c r="H262" s="7"/>
       <c r="I262" s="7"/>
-    </row>
-    <row r="263" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J262" s="7"/>
+      <c r="K262" s="7"/>
+    </row>
+    <row r="263" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="9"/>
       <c r="B263" s="9"/>
       <c r="C263" s="9"/>
@@ -4470,8 +5032,10 @@
       <c r="G263" s="7"/>
       <c r="H263" s="7"/>
       <c r="I263" s="7"/>
-    </row>
-    <row r="264" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J263" s="7"/>
+      <c r="K263" s="7"/>
+    </row>
+    <row r="264" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="9"/>
       <c r="B264" s="9"/>
       <c r="C264" s="9"/>
@@ -4481,8 +5045,10 @@
       <c r="G264" s="7"/>
       <c r="H264" s="7"/>
       <c r="I264" s="7"/>
-    </row>
-    <row r="265" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J264" s="7"/>
+      <c r="K264" s="7"/>
+    </row>
+    <row r="265" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="9"/>
       <c r="B265" s="9"/>
       <c r="C265" s="9"/>
@@ -4492,8 +5058,10 @@
       <c r="G265" s="7"/>
       <c r="H265" s="7"/>
       <c r="I265" s="7"/>
-    </row>
-    <row r="266" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J265" s="7"/>
+      <c r="K265" s="7"/>
+    </row>
+    <row r="266" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="9"/>
       <c r="B266" s="9"/>
       <c r="C266" s="9"/>
@@ -4503,8 +5071,10 @@
       <c r="G266" s="7"/>
       <c r="H266" s="7"/>
       <c r="I266" s="7"/>
-    </row>
-    <row r="267" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J266" s="7"/>
+      <c r="K266" s="7"/>
+    </row>
+    <row r="267" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="9"/>
       <c r="B267" s="9"/>
       <c r="C267" s="9"/>
@@ -4514,8 +5084,10 @@
       <c r="G267" s="7"/>
       <c r="H267" s="7"/>
       <c r="I267" s="7"/>
-    </row>
-    <row r="268" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J267" s="7"/>
+      <c r="K267" s="7"/>
+    </row>
+    <row r="268" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="9"/>
       <c r="B268" s="9"/>
       <c r="C268" s="9"/>
@@ -4525,8 +5097,10 @@
       <c r="G268" s="7"/>
       <c r="H268" s="7"/>
       <c r="I268" s="7"/>
-    </row>
-    <row r="269" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J268" s="7"/>
+      <c r="K268" s="7"/>
+    </row>
+    <row r="269" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="9"/>
       <c r="B269" s="9"/>
       <c r="C269" s="9"/>
@@ -4536,8 +5110,10 @@
       <c r="G269" s="7"/>
       <c r="H269" s="7"/>
       <c r="I269" s="7"/>
-    </row>
-    <row r="270" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J269" s="7"/>
+      <c r="K269" s="7"/>
+    </row>
+    <row r="270" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="9"/>
       <c r="B270" s="9"/>
       <c r="C270" s="9"/>
@@ -4547,8 +5123,10 @@
       <c r="G270" s="7"/>
       <c r="H270" s="7"/>
       <c r="I270" s="7"/>
-    </row>
-    <row r="271" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J270" s="7"/>
+      <c r="K270" s="7"/>
+    </row>
+    <row r="271" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="9"/>
       <c r="B271" s="9"/>
       <c r="C271" s="9"/>
@@ -4558,8 +5136,10 @@
       <c r="G271" s="7"/>
       <c r="H271" s="7"/>
       <c r="I271" s="7"/>
-    </row>
-    <row r="272" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J271" s="7"/>
+      <c r="K271" s="7"/>
+    </row>
+    <row r="272" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="9"/>
       <c r="B272" s="9"/>
       <c r="C272" s="9"/>
@@ -4569,8 +5149,10 @@
       <c r="G272" s="7"/>
       <c r="H272" s="7"/>
       <c r="I272" s="7"/>
-    </row>
-    <row r="273" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J272" s="7"/>
+      <c r="K272" s="7"/>
+    </row>
+    <row r="273" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="9"/>
       <c r="B273" s="9"/>
       <c r="C273" s="9"/>
@@ -4580,8 +5162,10 @@
       <c r="G273" s="7"/>
       <c r="H273" s="7"/>
       <c r="I273" s="7"/>
-    </row>
-    <row r="274" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J273" s="7"/>
+      <c r="K273" s="7"/>
+    </row>
+    <row r="274" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="9"/>
       <c r="B274" s="9"/>
       <c r="C274" s="9"/>
@@ -4591,8 +5175,10 @@
       <c r="G274" s="7"/>
       <c r="H274" s="7"/>
       <c r="I274" s="7"/>
-    </row>
-    <row r="275" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J274" s="7"/>
+      <c r="K274" s="7"/>
+    </row>
+    <row r="275" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="9"/>
       <c r="B275" s="9"/>
       <c r="C275" s="9"/>
@@ -4602,8 +5188,10 @@
       <c r="G275" s="7"/>
       <c r="H275" s="7"/>
       <c r="I275" s="7"/>
-    </row>
-    <row r="276" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J275" s="7"/>
+      <c r="K275" s="7"/>
+    </row>
+    <row r="276" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="9"/>
       <c r="B276" s="9"/>
       <c r="C276" s="9"/>
@@ -4613,8 +5201,10 @@
       <c r="G276" s="7"/>
       <c r="H276" s="7"/>
       <c r="I276" s="7"/>
-    </row>
-    <row r="277" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J276" s="7"/>
+      <c r="K276" s="7"/>
+    </row>
+    <row r="277" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="9"/>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
@@ -4624,8 +5214,10 @@
       <c r="G277" s="7"/>
       <c r="H277" s="7"/>
       <c r="I277" s="7"/>
-    </row>
-    <row r="278" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J277" s="7"/>
+      <c r="K277" s="7"/>
+    </row>
+    <row r="278" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="9"/>
       <c r="B278" s="9"/>
       <c r="C278" s="9"/>
@@ -4635,8 +5227,10 @@
       <c r="G278" s="7"/>
       <c r="H278" s="7"/>
       <c r="I278" s="7"/>
-    </row>
-    <row r="279" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J278" s="7"/>
+      <c r="K278" s="7"/>
+    </row>
+    <row r="279" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="9"/>
       <c r="B279" s="9"/>
       <c r="C279" s="9"/>
@@ -4646,8 +5240,10 @@
       <c r="G279" s="7"/>
       <c r="H279" s="7"/>
       <c r="I279" s="7"/>
-    </row>
-    <row r="280" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J279" s="7"/>
+      <c r="K279" s="7"/>
+    </row>
+    <row r="280" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="9"/>
       <c r="B280" s="9"/>
       <c r="C280" s="9"/>
@@ -4657,8 +5253,10 @@
       <c r="G280" s="7"/>
       <c r="H280" s="7"/>
       <c r="I280" s="7"/>
-    </row>
-    <row r="281" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J280" s="7"/>
+      <c r="K280" s="7"/>
+    </row>
+    <row r="281" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="9"/>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
@@ -4668,8 +5266,10 @@
       <c r="G281" s="7"/>
       <c r="H281" s="7"/>
       <c r="I281" s="7"/>
-    </row>
-    <row r="282" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J281" s="7"/>
+      <c r="K281" s="7"/>
+    </row>
+    <row r="282" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="9"/>
       <c r="B282" s="9"/>
       <c r="C282" s="9"/>
@@ -4679,8 +5279,10 @@
       <c r="G282" s="7"/>
       <c r="H282" s="7"/>
       <c r="I282" s="7"/>
-    </row>
-    <row r="283" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J282" s="7"/>
+      <c r="K282" s="7"/>
+    </row>
+    <row r="283" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="9"/>
       <c r="B283" s="9"/>
       <c r="C283" s="9"/>
@@ -4690,8 +5292,10 @@
       <c r="G283" s="7"/>
       <c r="H283" s="7"/>
       <c r="I283" s="7"/>
-    </row>
-    <row r="284" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J283" s="7"/>
+      <c r="K283" s="7"/>
+    </row>
+    <row r="284" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="9"/>
       <c r="B284" s="9"/>
       <c r="C284" s="9"/>
@@ -4701,8 +5305,10 @@
       <c r="G284" s="7"/>
       <c r="H284" s="7"/>
       <c r="I284" s="7"/>
-    </row>
-    <row r="285" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J284" s="7"/>
+      <c r="K284" s="7"/>
+    </row>
+    <row r="285" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="9"/>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
@@ -4712,8 +5318,10 @@
       <c r="G285" s="7"/>
       <c r="H285" s="7"/>
       <c r="I285" s="7"/>
-    </row>
-    <row r="286" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J285" s="7"/>
+      <c r="K285" s="7"/>
+    </row>
+    <row r="286" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="9"/>
       <c r="B286" s="9"/>
       <c r="C286" s="9"/>
@@ -4723,8 +5331,10 @@
       <c r="G286" s="7"/>
       <c r="H286" s="7"/>
       <c r="I286" s="7"/>
-    </row>
-    <row r="287" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J286" s="7"/>
+      <c r="K286" s="7"/>
+    </row>
+    <row r="287" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="9"/>
       <c r="B287" s="9"/>
       <c r="C287" s="9"/>
@@ -4734,8 +5344,10 @@
       <c r="G287" s="7"/>
       <c r="H287" s="7"/>
       <c r="I287" s="7"/>
-    </row>
-    <row r="288" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J287" s="7"/>
+      <c r="K287" s="7"/>
+    </row>
+    <row r="288" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="9"/>
       <c r="B288" s="9"/>
       <c r="C288" s="9"/>
@@ -4745,8 +5357,10 @@
       <c r="G288" s="7"/>
       <c r="H288" s="7"/>
       <c r="I288" s="7"/>
-    </row>
-    <row r="289" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J288" s="7"/>
+      <c r="K288" s="7"/>
+    </row>
+    <row r="289" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="9"/>
       <c r="B289" s="9"/>
       <c r="C289" s="9"/>
@@ -4756,8 +5370,10 @@
       <c r="G289" s="7"/>
       <c r="H289" s="7"/>
       <c r="I289" s="7"/>
-    </row>
-    <row r="290" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J289" s="7"/>
+      <c r="K289" s="7"/>
+    </row>
+    <row r="290" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="9"/>
       <c r="B290" s="9"/>
       <c r="C290" s="9"/>
@@ -4767,8 +5383,10 @@
       <c r="G290" s="7"/>
       <c r="H290" s="7"/>
       <c r="I290" s="7"/>
-    </row>
-    <row r="291" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J290" s="7"/>
+      <c r="K290" s="7"/>
+    </row>
+    <row r="291" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="9"/>
       <c r="B291" s="9"/>
       <c r="C291" s="9"/>
@@ -4778,8 +5396,10 @@
       <c r="G291" s="7"/>
       <c r="H291" s="7"/>
       <c r="I291" s="7"/>
-    </row>
-    <row r="292" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J291" s="7"/>
+      <c r="K291" s="7"/>
+    </row>
+    <row r="292" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="9"/>
       <c r="B292" s="9"/>
       <c r="C292" s="9"/>
@@ -4789,8 +5409,10 @@
       <c r="G292" s="7"/>
       <c r="H292" s="7"/>
       <c r="I292" s="7"/>
-    </row>
-    <row r="293" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J292" s="7"/>
+      <c r="K292" s="7"/>
+    </row>
+    <row r="293" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="9"/>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
@@ -4800,8 +5422,10 @@
       <c r="G293" s="7"/>
       <c r="H293" s="7"/>
       <c r="I293" s="7"/>
-    </row>
-    <row r="294" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J293" s="7"/>
+      <c r="K293" s="7"/>
+    </row>
+    <row r="294" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="9"/>
       <c r="B294" s="9"/>
       <c r="C294" s="9"/>
@@ -4811,8 +5435,10 @@
       <c r="G294" s="7"/>
       <c r="H294" s="7"/>
       <c r="I294" s="7"/>
-    </row>
-    <row r="295" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J294" s="7"/>
+      <c r="K294" s="7"/>
+    </row>
+    <row r="295" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="9"/>
       <c r="B295" s="9"/>
       <c r="C295" s="9"/>
@@ -4822,8 +5448,10 @@
       <c r="G295" s="7"/>
       <c r="H295" s="7"/>
       <c r="I295" s="7"/>
-    </row>
-    <row r="296" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J295" s="7"/>
+      <c r="K295" s="7"/>
+    </row>
+    <row r="296" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="9"/>
       <c r="B296" s="9"/>
       <c r="C296" s="9"/>
@@ -4833,8 +5461,10 @@
       <c r="G296" s="7"/>
       <c r="H296" s="7"/>
       <c r="I296" s="7"/>
-    </row>
-    <row r="297" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J296" s="7"/>
+      <c r="K296" s="7"/>
+    </row>
+    <row r="297" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="9"/>
       <c r="B297" s="9"/>
       <c r="C297" s="9"/>
@@ -4844,8 +5474,10 @@
       <c r="G297" s="7"/>
       <c r="H297" s="7"/>
       <c r="I297" s="7"/>
-    </row>
-    <row r="298" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J297" s="7"/>
+      <c r="K297" s="7"/>
+    </row>
+    <row r="298" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="9"/>
       <c r="B298" s="9"/>
       <c r="C298" s="9"/>
@@ -4855,8 +5487,10 @@
       <c r="G298" s="7"/>
       <c r="H298" s="7"/>
       <c r="I298" s="7"/>
-    </row>
-    <row r="299" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J298" s="7"/>
+      <c r="K298" s="7"/>
+    </row>
+    <row r="299" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="9"/>
       <c r="B299" s="9"/>
       <c r="C299" s="9"/>
@@ -4866,8 +5500,10 @@
       <c r="G299" s="7"/>
       <c r="H299" s="7"/>
       <c r="I299" s="7"/>
-    </row>
-    <row r="300" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J299" s="7"/>
+      <c r="K299" s="7"/>
+    </row>
+    <row r="300" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="9"/>
       <c r="B300" s="9"/>
       <c r="C300" s="9"/>
@@ -4877,8 +5513,10 @@
       <c r="G300" s="7"/>
       <c r="H300" s="7"/>
       <c r="I300" s="7"/>
-    </row>
-    <row r="301" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J300" s="7"/>
+      <c r="K300" s="7"/>
+    </row>
+    <row r="301" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="9"/>
       <c r="B301" s="9"/>
       <c r="C301" s="9"/>
@@ -4888,8 +5526,10 @@
       <c r="G301" s="7"/>
       <c r="H301" s="7"/>
       <c r="I301" s="7"/>
-    </row>
-    <row r="302" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J301" s="7"/>
+      <c r="K301" s="7"/>
+    </row>
+    <row r="302" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="9"/>
       <c r="B302" s="9"/>
       <c r="C302" s="9"/>
@@ -4899,8 +5539,10 @@
       <c r="G302" s="7"/>
       <c r="H302" s="7"/>
       <c r="I302" s="7"/>
-    </row>
-    <row r="303" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J302" s="7"/>
+      <c r="K302" s="7"/>
+    </row>
+    <row r="303" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="9"/>
       <c r="B303" s="9"/>
       <c r="C303" s="9"/>
@@ -4910,8 +5552,10 @@
       <c r="G303" s="7"/>
       <c r="H303" s="7"/>
       <c r="I303" s="7"/>
-    </row>
-    <row r="304" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J303" s="7"/>
+      <c r="K303" s="7"/>
+    </row>
+    <row r="304" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="9"/>
       <c r="B304" s="9"/>
       <c r="C304" s="9"/>
@@ -4921,8 +5565,10 @@
       <c r="G304" s="7"/>
       <c r="H304" s="7"/>
       <c r="I304" s="7"/>
-    </row>
-    <row r="305" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J304" s="7"/>
+      <c r="K304" s="7"/>
+    </row>
+    <row r="305" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="9"/>
       <c r="B305" s="9"/>
       <c r="C305" s="9"/>
@@ -4932,8 +5578,10 @@
       <c r="G305" s="7"/>
       <c r="H305" s="7"/>
       <c r="I305" s="7"/>
-    </row>
-    <row r="306" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J305" s="7"/>
+      <c r="K305" s="7"/>
+    </row>
+    <row r="306" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="9"/>
       <c r="B306" s="9"/>
       <c r="C306" s="9"/>
@@ -4943,8 +5591,10 @@
       <c r="G306" s="7"/>
       <c r="H306" s="7"/>
       <c r="I306" s="7"/>
-    </row>
-    <row r="307" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J306" s="7"/>
+      <c r="K306" s="7"/>
+    </row>
+    <row r="307" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="9"/>
       <c r="B307" s="9"/>
       <c r="C307" s="9"/>
@@ -4954,8 +5604,10 @@
       <c r="G307" s="7"/>
       <c r="H307" s="7"/>
       <c r="I307" s="7"/>
-    </row>
-    <row r="308" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J307" s="7"/>
+      <c r="K307" s="7"/>
+    </row>
+    <row r="308" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="9"/>
       <c r="B308" s="9"/>
       <c r="C308" s="9"/>
@@ -4965,8 +5617,10 @@
       <c r="G308" s="7"/>
       <c r="H308" s="7"/>
       <c r="I308" s="7"/>
-    </row>
-    <row r="309" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J308" s="7"/>
+      <c r="K308" s="7"/>
+    </row>
+    <row r="309" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="9"/>
       <c r="B309" s="9"/>
       <c r="C309" s="9"/>
@@ -4976,8 +5630,10 @@
       <c r="G309" s="7"/>
       <c r="H309" s="7"/>
       <c r="I309" s="7"/>
-    </row>
-    <row r="310" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J309" s="7"/>
+      <c r="K309" s="7"/>
+    </row>
+    <row r="310" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="9"/>
       <c r="B310" s="9"/>
       <c r="C310" s="9"/>
@@ -4987,8 +5643,10 @@
       <c r="G310" s="7"/>
       <c r="H310" s="7"/>
       <c r="I310" s="7"/>
-    </row>
-    <row r="311" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J310" s="7"/>
+      <c r="K310" s="7"/>
+    </row>
+    <row r="311" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="9"/>
       <c r="B311" s="9"/>
       <c r="C311" s="9"/>
@@ -4998,8 +5656,10 @@
       <c r="G311" s="7"/>
       <c r="H311" s="7"/>
       <c r="I311" s="7"/>
-    </row>
-    <row r="312" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J311" s="7"/>
+      <c r="K311" s="7"/>
+    </row>
+    <row r="312" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="9"/>
       <c r="B312" s="9"/>
       <c r="C312" s="9"/>
@@ -5009,8 +5669,10 @@
       <c r="G312" s="7"/>
       <c r="H312" s="7"/>
       <c r="I312" s="7"/>
-    </row>
-    <row r="313" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J312" s="7"/>
+      <c r="K312" s="7"/>
+    </row>
+    <row r="313" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="9"/>
       <c r="B313" s="9"/>
       <c r="C313" s="9"/>
@@ -5020,8 +5682,10 @@
       <c r="G313" s="7"/>
       <c r="H313" s="7"/>
       <c r="I313" s="7"/>
-    </row>
-    <row r="314" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J313" s="7"/>
+      <c r="K313" s="7"/>
+    </row>
+    <row r="314" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="9"/>
       <c r="B314" s="9"/>
       <c r="C314" s="9"/>
@@ -5031,8 +5695,10 @@
       <c r="G314" s="7"/>
       <c r="H314" s="7"/>
       <c r="I314" s="7"/>
-    </row>
-    <row r="315" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J314" s="7"/>
+      <c r="K314" s="7"/>
+    </row>
+    <row r="315" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="9"/>
       <c r="B315" s="9"/>
       <c r="C315" s="9"/>
@@ -5042,8 +5708,10 @@
       <c r="G315" s="7"/>
       <c r="H315" s="7"/>
       <c r="I315" s="7"/>
-    </row>
-    <row r="316" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J315" s="7"/>
+      <c r="K315" s="7"/>
+    </row>
+    <row r="316" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="9"/>
       <c r="B316" s="9"/>
       <c r="C316" s="9"/>
@@ -5053,8 +5721,10 @@
       <c r="G316" s="7"/>
       <c r="H316" s="7"/>
       <c r="I316" s="7"/>
-    </row>
-    <row r="317" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J316" s="7"/>
+      <c r="K316" s="7"/>
+    </row>
+    <row r="317" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="9"/>
       <c r="B317" s="9"/>
       <c r="C317" s="9"/>
@@ -5064,8 +5734,10 @@
       <c r="G317" s="7"/>
       <c r="H317" s="7"/>
       <c r="I317" s="7"/>
-    </row>
-    <row r="318" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J317" s="7"/>
+      <c r="K317" s="7"/>
+    </row>
+    <row r="318" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="9"/>
       <c r="B318" s="9"/>
       <c r="C318" s="9"/>
@@ -5075,8 +5747,10 @@
       <c r="G318" s="7"/>
       <c r="H318" s="7"/>
       <c r="I318" s="7"/>
-    </row>
-    <row r="319" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J318" s="7"/>
+      <c r="K318" s="7"/>
+    </row>
+    <row r="319" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="9"/>
       <c r="B319" s="9"/>
       <c r="C319" s="9"/>
@@ -5086,8 +5760,10 @@
       <c r="G319" s="7"/>
       <c r="H319" s="7"/>
       <c r="I319" s="7"/>
-    </row>
-    <row r="320" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J319" s="7"/>
+      <c r="K319" s="7"/>
+    </row>
+    <row r="320" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="9"/>
       <c r="B320" s="9"/>
       <c r="C320" s="9"/>
@@ -5097,8 +5773,10 @@
       <c r="G320" s="7"/>
       <c r="H320" s="7"/>
       <c r="I320" s="7"/>
-    </row>
-    <row r="321" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J320" s="7"/>
+      <c r="K320" s="7"/>
+    </row>
+    <row r="321" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="9"/>
       <c r="B321" s="9"/>
       <c r="C321" s="9"/>
@@ -5108,8 +5786,10 @@
       <c r="G321" s="7"/>
       <c r="H321" s="7"/>
       <c r="I321" s="7"/>
-    </row>
-    <row r="322" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J321" s="7"/>
+      <c r="K321" s="7"/>
+    </row>
+    <row r="322" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="9"/>
       <c r="B322" s="9"/>
       <c r="C322" s="9"/>
@@ -5119,8 +5799,10 @@
       <c r="G322" s="7"/>
       <c r="H322" s="7"/>
       <c r="I322" s="7"/>
-    </row>
-    <row r="323" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J322" s="7"/>
+      <c r="K322" s="7"/>
+    </row>
+    <row r="323" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="9"/>
       <c r="B323" s="9"/>
       <c r="C323" s="9"/>
@@ -5130,8 +5812,11 @@
       <c r="G323" s="7"/>
       <c r="H323" s="7"/>
       <c r="I323" s="7"/>
+      <c r="J323" s="7"/>
+      <c r="K323" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>